<commit_message>
Continuing work on excel import
</commit_message>
<xml_diff>
--- a/example-import-data.xlsx
+++ b/example-import-data.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="2140" windowWidth="38540" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="6120" yWindow="2000" windowWidth="42680" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="example-csv.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="162">
   <si>
     <t>Name</t>
   </si>
@@ -502,20 +502,40 @@
     <t>Date</t>
   </si>
   <si>
-    <t>DD/MM/YY</t>
+    <t>Test Date</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -538,15 +558,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -876,1692 +910,1780 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W25"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="20" max="20" width="29.6640625" customWidth="1"/>
-    <col min="21" max="21" width="19.83203125" customWidth="1"/>
-    <col min="22" max="22" width="20.1640625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="17" max="17" width="17" style="3" customWidth="1"/>
+    <col min="20" max="20" width="16.1640625" customWidth="1"/>
+    <col min="21" max="21" width="16.1640625" style="4" customWidth="1"/>
+    <col min="22" max="22" width="16.6640625" customWidth="1"/>
+    <col min="24" max="24" width="29.6640625" customWidth="1"/>
+    <col min="25" max="25" width="19.83203125" customWidth="1"/>
+    <col min="26" max="26" width="20.1640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>159</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>160</v>
-      </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2">
+        <v>40706</v>
+      </c>
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>4060</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>403844972</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="L2">
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="O2">
         <v>99</v>
       </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
         <v>101.15</v>
       </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
         <v>28</v>
       </c>
-      <c r="Q2">
+      <c r="T2">
         <v>11.9</v>
       </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="U2" t="s">
-        <v>29</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W2" s="2">
-        <v>40706</v>
+      <c r="U2" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>31</v>
       </c>
       <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="2">
+        <v>40707</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>36</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>4005</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>402838545</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
       <c r="M3">
         <v>0</v>
       </c>
-      <c r="N3">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
         <v>68</v>
       </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3" t="s">
         <v>37</v>
       </c>
-      <c r="Q3">
+      <c r="T3">
         <v>12</v>
       </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="U3" t="s">
-        <v>38</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="W3" s="2">
-        <v>40707</v>
+      <c r="U3" s="4">
+        <v>0.1021</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>40</v>
       </c>
       <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="2">
+        <v>40708</v>
+      </c>
+      <c r="E4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>43</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>44</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>45</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>27</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>4069</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>432431162</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="L4">
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="O4">
         <v>139</v>
       </c>
-      <c r="M4">
+      <c r="P4">
         <v>85</v>
       </c>
-      <c r="N4">
+      <c r="Q4" s="3">
         <v>241.4</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4" t="s">
         <v>28</v>
       </c>
-      <c r="Q4">
+      <c r="T4">
         <v>42.6</v>
       </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="U4" t="s">
-        <v>46</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="W4" s="2">
-        <v>40708</v>
+      <c r="U4" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>48</v>
       </c>
       <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="2">
+        <v>40709</v>
+      </c>
+      <c r="E5" t="s">
         <v>49</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>50</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>52</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>53</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>27</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>4170</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <v>417699448</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="L5">
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="O5">
         <v>60</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
         <v>51</v>
       </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" t="s">
         <v>37</v>
       </c>
-      <c r="Q5">
+      <c r="T5">
         <v>9</v>
       </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="U5" t="s">
-        <v>54</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="W5" s="2">
-        <v>40709</v>
+      <c r="U5" s="4">
+        <v>0.23566999999999999</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>56</v>
       </c>
       <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="2">
+        <v>40710</v>
+      </c>
+      <c r="E6" t="s">
         <v>57</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>58</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
         <v>60</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
         <v>27</v>
       </c>
-      <c r="H6">
+      <c r="K6">
         <v>4152</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>438808849</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="L6">
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="O6">
         <v>139</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
         <v>139</v>
       </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" t="s">
         <v>28</v>
       </c>
-      <c r="Q6">
+      <c r="T6">
         <v>29.85</v>
       </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6" t="s">
+      <c r="U6" s="4">
+        <v>0.46550000000000002</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6" t="s">
         <v>61</v>
       </c>
-      <c r="U6" t="s">
-        <v>62</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="W6" s="2">
-        <v>40710</v>
-      </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>64</v>
       </c>
       <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2">
+        <v>40711</v>
+      </c>
+      <c r="E7" t="s">
         <v>65</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>66</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>67</v>
       </c>
-      <c r="F7" t="s">
+      <c r="I7" t="s">
         <v>68</v>
       </c>
-      <c r="G7" t="s">
+      <c r="J7" t="s">
         <v>27</v>
       </c>
-      <c r="H7">
+      <c r="K7">
         <v>4152</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <v>433461842</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
         <v>80</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7" t="s">
         <v>37</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="U7" t="s">
-        <v>69</v>
-      </c>
-      <c r="W7" s="2">
-        <v>40711</v>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7" s="4">
+        <v>0.48602499999999998</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
         <v>70</v>
       </c>
       <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="2">
+        <v>40712</v>
+      </c>
+      <c r="E8" t="s">
         <v>71</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>72</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>73</v>
       </c>
-      <c r="F8" t="s">
+      <c r="I8" t="s">
         <v>74</v>
       </c>
-      <c r="G8" t="s">
+      <c r="J8" t="s">
         <v>27</v>
       </c>
-      <c r="H8">
+      <c r="K8">
         <v>4171</v>
       </c>
-      <c r="I8">
+      <c r="L8">
         <v>418727030</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="L8">
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="O8">
         <v>400</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
         <v>320</v>
       </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" t="s">
         <v>37</v>
       </c>
-      <c r="Q8">
+      <c r="T8">
         <v>60</v>
       </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8" t="s">
+      <c r="U8" s="4">
+        <v>0.57248200000000005</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8" t="s">
         <v>75</v>
       </c>
-      <c r="U8" t="s">
-        <v>76</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="W8" s="2">
-        <v>40712</v>
-      </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
         <v>78</v>
       </c>
       <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="2">
+        <v>40713</v>
+      </c>
+      <c r="E9" t="s">
         <v>79</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>80</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>81</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
         <v>82</v>
       </c>
-      <c r="F9" t="s">
+      <c r="I9" t="s">
         <v>83</v>
       </c>
-      <c r="G9" t="s">
+      <c r="J9" t="s">
         <v>27</v>
       </c>
-      <c r="H9">
+      <c r="K9">
         <v>4151</v>
       </c>
-      <c r="I9">
+      <c r="L9">
         <v>435511522</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="L9">
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="O9">
         <v>119</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
         <v>125.1</v>
       </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9" t="s">
         <v>28</v>
       </c>
-      <c r="Q9">
+      <c r="T9">
         <v>13.9</v>
       </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="U9" t="s">
-        <v>84</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="W9" s="2">
-        <v>40713</v>
+      <c r="U9" s="4">
+        <v>0.65893900000000005</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:24">
       <c r="A10" t="s">
         <v>86</v>
       </c>
       <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="2">
+        <v>40714</v>
+      </c>
+      <c r="E10" t="s">
         <v>87</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
         <v>88</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10" t="s">
         <v>89</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>90</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I10" t="s">
         <v>91</v>
       </c>
-      <c r="G10" t="s">
+      <c r="J10" t="s">
         <v>27</v>
       </c>
-      <c r="H10">
+      <c r="K10">
         <v>4011</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <v>447001140</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="L10">
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="O10">
         <v>119</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3">
         <v>159</v>
       </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" t="s">
         <v>28</v>
       </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="U10" t="s">
-        <v>92</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="W10" s="2">
-        <v>40714</v>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10" s="4">
+        <v>0.74539599999999995</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:24">
       <c r="A11" t="s">
         <v>94</v>
       </c>
       <c r="B11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="2">
+        <v>40715</v>
+      </c>
+      <c r="E11" t="s">
         <v>95</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>96</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
         <v>97</v>
       </c>
-      <c r="E11" t="s">
+      <c r="H11" t="s">
         <v>98</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I11" t="s">
         <v>99</v>
       </c>
-      <c r="G11" t="s">
+      <c r="J11" t="s">
         <v>27</v>
       </c>
-      <c r="H11">
+      <c r="K11">
         <v>4007</v>
       </c>
-      <c r="I11">
+      <c r="L11">
         <v>410362988</v>
       </c>
-      <c r="J11">
+      <c r="M11">
         <v>2</v>
       </c>
-      <c r="L11">
+      <c r="O11">
         <v>100</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3">
         <v>85</v>
       </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11" t="s">
         <v>28</v>
       </c>
-      <c r="Q11">
+      <c r="T11">
         <v>15</v>
       </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11" t="s">
+      <c r="U11" s="4">
+        <v>0.83185299999999995</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11" t="s">
         <v>61</v>
       </c>
-      <c r="U11" t="s">
-        <v>100</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="W11" s="2">
-        <v>40715</v>
-      </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:24">
       <c r="A12" t="s">
         <v>102</v>
       </c>
       <c r="B12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2">
+        <v>40716</v>
+      </c>
+      <c r="E12" t="s">
         <v>103</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>104</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G12" t="s">
         <v>105</v>
       </c>
-      <c r="E12" t="s">
+      <c r="H12" t="s">
         <v>106</v>
       </c>
-      <c r="F12" t="s">
+      <c r="I12" t="s">
         <v>107</v>
       </c>
-      <c r="G12" t="s">
+      <c r="J12" t="s">
         <v>27</v>
       </c>
-      <c r="H12">
+      <c r="K12">
         <v>4121</v>
       </c>
-      <c r="I12">
+      <c r="L12">
         <v>402707887</v>
       </c>
-      <c r="J12">
+      <c r="M12">
         <v>2</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3">
         <v>160</v>
       </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12" t="s">
         <v>37</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12" t="s">
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12" s="4">
+        <v>0.91830999999999996</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12" t="s">
         <v>61</v>
       </c>
-      <c r="U12" t="s">
-        <v>108</v>
-      </c>
-      <c r="W12" s="2">
-        <v>40716</v>
-      </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:24">
       <c r="A13" t="s">
         <v>30</v>
       </c>
       <c r="B13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="2">
+        <v>40717</v>
+      </c>
+      <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
+      <c r="F13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
+      <c r="G13" t="s">
         <v>24</v>
       </c>
-      <c r="E13" t="s">
+      <c r="H13" t="s">
         <v>25</v>
       </c>
-      <c r="F13" t="s">
+      <c r="I13" t="s">
         <v>26</v>
       </c>
-      <c r="G13" t="s">
+      <c r="J13" t="s">
         <v>27</v>
       </c>
-      <c r="H13">
+      <c r="K13">
         <v>4060</v>
       </c>
-      <c r="I13">
+      <c r="L13">
         <v>403844972</v>
       </c>
-      <c r="J13">
+      <c r="M13">
         <v>2</v>
       </c>
-      <c r="K13" t="s">
+      <c r="N13" t="s">
         <v>109</v>
       </c>
-      <c r="L13">
+      <c r="O13">
         <v>169</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3">
         <v>177.65</v>
       </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13" t="s">
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13" t="s">
         <v>28</v>
       </c>
-      <c r="Q13">
+      <c r="T13">
         <v>20.9</v>
       </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13" t="s">
+      <c r="U13" s="4">
+        <v>1.004767</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13" t="s">
         <v>61</v>
       </c>
-      <c r="U13" t="s">
-        <v>110</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="W13" s="2">
-        <v>40717</v>
-      </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:24">
       <c r="A14" t="s">
         <v>112</v>
       </c>
       <c r="B14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2">
+        <v>40718</v>
+      </c>
+      <c r="E14" t="s">
         <v>113</v>
       </c>
-      <c r="C14" t="s">
+      <c r="F14" t="s">
         <v>114</v>
       </c>
-      <c r="D14" t="s">
+      <c r="G14" t="s">
         <v>115</v>
       </c>
-      <c r="E14" t="s">
+      <c r="H14" t="s">
         <v>116</v>
       </c>
-      <c r="F14" t="s">
+      <c r="I14" t="s">
         <v>117</v>
       </c>
-      <c r="G14" t="s">
+      <c r="J14" t="s">
         <v>27</v>
       </c>
-      <c r="H14">
+      <c r="K14">
         <v>4508</v>
       </c>
-      <c r="I14">
+      <c r="L14">
         <v>42566047</v>
       </c>
-      <c r="J14">
+      <c r="M14">
         <v>2</v>
       </c>
-      <c r="K14" t="s">
+      <c r="N14" t="s">
         <v>118</v>
       </c>
-      <c r="L14">
+      <c r="O14">
         <v>139</v>
       </c>
-      <c r="M14">
+      <c r="P14">
         <v>300</v>
       </c>
-      <c r="N14">
+      <c r="Q14" s="3">
         <v>350</v>
       </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14" t="s">
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14" t="s">
         <v>28</v>
       </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14" t="s">
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14" s="4">
+        <v>1.091224</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14" t="s">
         <v>119</v>
       </c>
-      <c r="U14" t="s">
-        <v>120</v>
-      </c>
-      <c r="W14" s="2">
-        <v>40718</v>
-      </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:24">
       <c r="A15" t="s">
         <v>39</v>
       </c>
       <c r="B15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="2">
+        <v>40719</v>
+      </c>
+      <c r="E15" t="s">
         <v>32</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F15" t="s">
         <v>33</v>
       </c>
-      <c r="D15" t="s">
+      <c r="G15" t="s">
         <v>34</v>
       </c>
-      <c r="E15" t="s">
+      <c r="H15" t="s">
         <v>35</v>
       </c>
-      <c r="F15" t="s">
+      <c r="I15" t="s">
         <v>36</v>
       </c>
-      <c r="G15" t="s">
+      <c r="J15" t="s">
         <v>27</v>
       </c>
-      <c r="H15">
+      <c r="K15">
         <v>4005</v>
       </c>
-      <c r="I15">
+      <c r="L15">
         <v>402838545</v>
       </c>
-      <c r="J15">
+      <c r="M15">
         <v>2</v>
       </c>
-      <c r="K15" t="s">
+      <c r="N15" t="s">
         <v>121</v>
       </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="3">
         <v>68</v>
       </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15" t="s">
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15" t="s">
         <v>37</v>
       </c>
-      <c r="Q15">
+      <c r="T15">
         <v>12</v>
       </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15" t="s">
+      <c r="U15" s="4">
+        <v>1.177681</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15" t="s">
         <v>61</v>
       </c>
-      <c r="U15" t="s">
-        <v>122</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="W15" s="2">
-        <v>40719</v>
-      </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:24">
       <c r="A16" t="s">
         <v>47</v>
       </c>
       <c r="B16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="2">
+        <v>40720</v>
+      </c>
+      <c r="E16" t="s">
         <v>41</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F16" t="s">
         <v>42</v>
       </c>
-      <c r="D16" t="s">
+      <c r="G16" t="s">
         <v>43</v>
       </c>
-      <c r="E16" t="s">
+      <c r="H16" t="s">
         <v>44</v>
       </c>
-      <c r="F16" t="s">
+      <c r="I16" t="s">
         <v>45</v>
       </c>
-      <c r="G16" t="s">
+      <c r="J16" t="s">
         <v>27</v>
       </c>
-      <c r="H16">
+      <c r="K16">
         <v>4069</v>
       </c>
-      <c r="I16">
+      <c r="L16">
         <v>432431162</v>
       </c>
-      <c r="J16">
+      <c r="M16">
         <v>2</v>
       </c>
-      <c r="K16" t="s">
+      <c r="N16" t="s">
         <v>124</v>
       </c>
-      <c r="L16">
+      <c r="O16">
         <v>139</v>
       </c>
-      <c r="M16">
+      <c r="P16">
         <v>25</v>
       </c>
-      <c r="N16">
+      <c r="Q16" s="3">
         <v>207.4</v>
       </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16" t="s">
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16" t="s">
         <v>28</v>
       </c>
-      <c r="Q16">
+      <c r="T16">
         <v>36.6</v>
       </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16" t="s">
+      <c r="U16" s="4">
+        <v>1.264138</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16" t="s">
         <v>61</v>
       </c>
-      <c r="U16" t="s">
-        <v>125</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="W16" s="2">
-        <v>40720</v>
-      </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:24">
       <c r="A17" t="s">
         <v>127</v>
       </c>
       <c r="B17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2">
+        <v>40721</v>
+      </c>
+      <c r="E17" t="s">
         <v>128</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
         <v>129</v>
       </c>
-      <c r="D17" t="s">
+      <c r="G17" t="s">
         <v>130</v>
       </c>
-      <c r="E17" t="s">
+      <c r="H17" t="s">
         <v>131</v>
       </c>
-      <c r="F17" t="s">
+      <c r="I17" t="s">
         <v>132</v>
       </c>
-      <c r="G17" t="s">
+      <c r="J17" t="s">
         <v>27</v>
       </c>
-      <c r="H17">
+      <c r="K17">
         <v>4006</v>
       </c>
-      <c r="I17">
+      <c r="L17">
         <v>412895591</v>
       </c>
-      <c r="J17">
+      <c r="M17">
         <v>2</v>
       </c>
-      <c r="L17">
+      <c r="O17">
         <v>119</v>
       </c>
-      <c r="M17">
+      <c r="P17">
         <v>440</v>
       </c>
-      <c r="N17">
+      <c r="Q17" s="3">
         <v>260</v>
       </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17" t="s">
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17" t="s">
         <v>28</v>
       </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17" t="s">
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17" s="4">
+        <v>1.350595</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17" t="s">
         <v>133</v>
       </c>
-      <c r="U17" t="s">
-        <v>134</v>
-      </c>
-      <c r="W17" s="2">
-        <v>40721</v>
-      </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:24">
       <c r="A18" t="s">
         <v>63</v>
       </c>
       <c r="B18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="2">
+        <v>40722</v>
+      </c>
+      <c r="E18" t="s">
         <v>57</v>
       </c>
-      <c r="D18" t="s">
+      <c r="G18" t="s">
         <v>58</v>
       </c>
-      <c r="E18" t="s">
+      <c r="H18" t="s">
         <v>59</v>
       </c>
-      <c r="F18" t="s">
+      <c r="I18" t="s">
         <v>60</v>
       </c>
-      <c r="G18" t="s">
+      <c r="J18" t="s">
         <v>27</v>
       </c>
-      <c r="H18">
+      <c r="K18">
         <v>4152</v>
       </c>
-      <c r="I18">
+      <c r="L18">
         <v>438808849</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="L18">
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="O18">
         <v>139</v>
       </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3">
         <v>139</v>
       </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18" t="s">
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18" t="s">
         <v>28</v>
       </c>
-      <c r="Q18">
+      <c r="T18">
         <v>29.85</v>
       </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18" t="s">
+      <c r="U18" s="4">
+        <v>1.437052</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18" t="s">
         <v>61</v>
       </c>
-      <c r="U18" t="s">
-        <v>135</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="W18" s="2">
-        <v>40722</v>
-      </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:24">
       <c r="A19" t="s">
         <v>137</v>
       </c>
       <c r="B19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="2">
+        <v>40723</v>
+      </c>
+      <c r="E19" t="s">
         <v>138</v>
       </c>
-      <c r="C19" t="s">
+      <c r="F19" t="s">
         <v>139</v>
       </c>
-      <c r="D19" t="s">
+      <c r="G19" t="s">
         <v>140</v>
       </c>
-      <c r="E19" t="s">
+      <c r="H19" t="s">
         <v>141</v>
       </c>
-      <c r="F19" t="s">
+      <c r="I19" t="s">
         <v>142</v>
       </c>
-      <c r="G19" t="s">
+      <c r="J19" t="s">
         <v>27</v>
       </c>
-      <c r="H19">
+      <c r="K19">
         <v>4069</v>
       </c>
-      <c r="I19">
+      <c r="L19">
         <v>402102872</v>
       </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="L19">
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="O19">
         <v>169</v>
       </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="3">
         <v>183.2</v>
       </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19" t="s">
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19" t="s">
         <v>28</v>
       </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-      <c r="T19" t="s">
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19" s="4">
+        <v>1.523509</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19" t="s">
         <v>75</v>
       </c>
-      <c r="U19" t="s">
-        <v>143</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="W19" s="2">
-        <v>40723</v>
-      </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:24">
       <c r="A20" t="s">
         <v>77</v>
       </c>
       <c r="B20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="2">
+        <v>40724</v>
+      </c>
+      <c r="E20" t="s">
         <v>71</v>
       </c>
-      <c r="D20" t="s">
+      <c r="G20" t="s">
         <v>72</v>
       </c>
-      <c r="E20" t="s">
+      <c r="H20" t="s">
         <v>73</v>
       </c>
-      <c r="F20" t="s">
+      <c r="I20" t="s">
         <v>74</v>
       </c>
-      <c r="G20" t="s">
+      <c r="J20" t="s">
         <v>27</v>
       </c>
-      <c r="H20">
+      <c r="K20">
         <v>4171</v>
       </c>
-      <c r="I20">
+      <c r="L20">
         <v>418727030</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="L20">
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="O20">
         <v>400</v>
       </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="3">
         <v>320</v>
       </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20" t="s">
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20" t="s">
         <v>37</v>
       </c>
-      <c r="Q20">
+      <c r="T20">
         <v>60</v>
       </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20" t="s">
+      <c r="U20" s="4">
+        <v>1.609966</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20" t="s">
         <v>75</v>
       </c>
-      <c r="U20" t="s">
-        <v>145</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="W20" s="2">
-        <v>40724</v>
-      </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:24">
       <c r="A21" t="s">
         <v>55</v>
       </c>
       <c r="B21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" s="2">
+        <v>40725</v>
+      </c>
+      <c r="E21" t="s">
         <v>49</v>
       </c>
-      <c r="C21" t="s">
+      <c r="F21" t="s">
         <v>50</v>
       </c>
-      <c r="D21" t="s">
+      <c r="G21" t="s">
         <v>51</v>
       </c>
-      <c r="E21" t="s">
+      <c r="H21" t="s">
         <v>52</v>
       </c>
-      <c r="F21" t="s">
+      <c r="I21" t="s">
         <v>53</v>
       </c>
-      <c r="G21" t="s">
+      <c r="J21" t="s">
         <v>27</v>
       </c>
-      <c r="H21">
+      <c r="K21">
         <v>4170</v>
       </c>
-      <c r="I21">
+      <c r="L21">
         <v>417699448</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="L21">
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="O21">
         <v>139</v>
       </c>
-      <c r="M21">
+      <c r="P21">
         <v>60</v>
       </c>
-      <c r="N21">
+      <c r="Q21" s="3">
         <v>186.15</v>
       </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21" t="s">
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21" t="s">
         <v>37</v>
       </c>
-      <c r="Q21">
+      <c r="T21">
         <v>32.85</v>
       </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21" t="s">
+      <c r="U21" s="4">
+        <v>1.696423</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21" t="s">
         <v>147</v>
       </c>
-      <c r="U21" t="s">
-        <v>148</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="W21" s="2">
-        <v>40725</v>
-      </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:24">
       <c r="A22" t="s">
         <v>101</v>
       </c>
       <c r="B22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" s="2">
+        <v>40726</v>
+      </c>
+      <c r="E22" t="s">
         <v>95</v>
       </c>
-      <c r="C22" t="s">
+      <c r="F22" t="s">
         <v>96</v>
       </c>
-      <c r="D22" t="s">
+      <c r="G22" t="s">
         <v>97</v>
       </c>
-      <c r="E22" t="s">
+      <c r="H22" t="s">
         <v>98</v>
       </c>
-      <c r="F22" t="s">
+      <c r="I22" t="s">
         <v>99</v>
       </c>
-      <c r="G22" t="s">
+      <c r="J22" t="s">
         <v>27</v>
       </c>
-      <c r="H22">
+      <c r="K22">
         <v>4007</v>
       </c>
-      <c r="I22">
+      <c r="L22">
         <v>410362988</v>
       </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="L22">
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="O22">
         <v>100</v>
       </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
         <v>85</v>
       </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22" t="s">
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22" t="s">
         <v>28</v>
       </c>
-      <c r="Q22">
+      <c r="T22">
         <v>15</v>
       </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22" t="s">
+      <c r="U22" s="4">
+        <v>1.78288</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22" t="s">
         <v>61</v>
       </c>
-      <c r="U22" t="s">
-        <v>150</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="W22" s="2">
-        <v>40726</v>
-      </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:24">
       <c r="A23" t="s">
         <v>144</v>
       </c>
       <c r="B23" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="2">
+        <v>40727</v>
+      </c>
+      <c r="E23" t="s">
         <v>138</v>
       </c>
-      <c r="C23" t="s">
+      <c r="F23" t="s">
         <v>139</v>
       </c>
-      <c r="D23" t="s">
+      <c r="G23" t="s">
         <v>140</v>
       </c>
-      <c r="E23" t="s">
+      <c r="H23" t="s">
         <v>141</v>
       </c>
-      <c r="F23" t="s">
+      <c r="I23" t="s">
         <v>142</v>
       </c>
-      <c r="G23" t="s">
+      <c r="J23" t="s">
         <v>27</v>
       </c>
-      <c r="H23">
+      <c r="K23">
         <v>4069</v>
       </c>
-      <c r="I23">
+      <c r="L23">
         <v>402102872</v>
       </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="L23">
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="O23">
         <v>169</v>
       </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3">
         <v>183.2</v>
       </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23" t="s">
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23" t="s">
         <v>28</v>
       </c>
-      <c r="Q23">
+      <c r="T23">
         <v>45.8</v>
       </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-      <c r="T23" t="s">
+      <c r="U23" s="4">
+        <v>1.869337</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23" t="s">
         <v>61</v>
       </c>
-      <c r="U23" t="s">
-        <v>152</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="W23" s="2">
-        <v>40727</v>
-      </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:24">
       <c r="A24" t="s">
         <v>111</v>
       </c>
       <c r="B24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" s="2">
+        <v>40728</v>
+      </c>
+      <c r="E24" t="s">
         <v>22</v>
       </c>
-      <c r="C24" t="s">
+      <c r="F24" t="s">
         <v>23</v>
       </c>
-      <c r="D24" t="s">
+      <c r="G24" t="s">
         <v>24</v>
       </c>
-      <c r="E24" t="s">
+      <c r="H24" t="s">
         <v>25</v>
       </c>
-      <c r="F24" t="s">
+      <c r="I24" t="s">
         <v>26</v>
       </c>
-      <c r="G24" t="s">
+      <c r="J24" t="s">
         <v>27</v>
       </c>
-      <c r="H24">
+      <c r="K24">
         <v>4060</v>
       </c>
-      <c r="I24">
+      <c r="L24">
         <v>403844972</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="L24">
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="O24">
         <v>99</v>
       </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="3">
         <v>101.15</v>
       </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24" t="s">
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24" t="s">
         <v>28</v>
       </c>
-      <c r="Q24">
+      <c r="T24">
         <v>11.9</v>
       </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24" t="s">
+      <c r="U24" s="4">
+        <v>1.955794</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24" t="s">
         <v>61</v>
       </c>
-      <c r="U24" t="s">
-        <v>154</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="W24" s="2">
-        <v>40728</v>
-      </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:24">
       <c r="A25" t="s">
         <v>123</v>
       </c>
       <c r="B25" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="2">
+        <v>40729</v>
+      </c>
+      <c r="E25" t="s">
         <v>32</v>
       </c>
-      <c r="C25" t="s">
+      <c r="F25" t="s">
         <v>33</v>
       </c>
-      <c r="D25" t="s">
+      <c r="G25" t="s">
         <v>34</v>
       </c>
-      <c r="E25" t="s">
+      <c r="H25" t="s">
         <v>35</v>
       </c>
-      <c r="F25" t="s">
+      <c r="I25" t="s">
         <v>36</v>
       </c>
-      <c r="G25" t="s">
+      <c r="J25" t="s">
         <v>27</v>
       </c>
-      <c r="H25">
+      <c r="K25">
         <v>4005</v>
       </c>
-      <c r="I25">
+      <c r="L25">
         <v>402838545</v>
       </c>
-      <c r="J25">
+      <c r="M25">
         <v>2</v>
       </c>
-      <c r="K25" t="s">
+      <c r="N25" t="s">
         <v>156</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25">
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="3">
         <v>68</v>
       </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25" t="s">
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25" t="s">
         <v>37</v>
       </c>
-      <c r="Q25">
+      <c r="T25">
         <v>12</v>
       </c>
-      <c r="R25">
-        <v>0</v>
-      </c>
-      <c r="S25">
-        <v>0</v>
-      </c>
-      <c r="T25" t="s">
+      <c r="U25" s="4">
+        <v>2.0422509999999998</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25" t="s">
         <v>61</v>
-      </c>
-      <c r="U25" t="s">
-        <v>157</v>
-      </c>
-      <c r="V25" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="W25" s="2">
-        <v>40729</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>